<commit_message>
feat[graficos]: criando um grafico lucro x gasto
</commit_message>
<xml_diff>
--- a/Automação/files/chart.xlsx
+++ b/Automação/files/chart.xlsx
@@ -149,6 +149,11 @@
         <ser>
           <idx val="0"/>
           <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Sheet'!C1</f>
+            </strRef>
+          </tx>
           <spPr>
             <a:ln>
               <a:prstDash val="solid"/>
@@ -156,18 +161,23 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$1:$A$7</f>
+              <f>'Sheet'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$B$1:$B$7</f>
+              <f>'Sheet'!$C$2:$C$7</f>
             </numRef>
           </val>
         </ser>
         <ser>
           <idx val="1"/>
           <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'Sheet'!B1</f>
+            </strRef>
+          </tx>
           <spPr>
             <a:ln>
               <a:prstDash val="solid"/>
@@ -175,12 +185,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$1:$A$7</f>
+              <f>'Sheet'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$C$1:$C$7</f>
+              <f>'Sheet'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -229,7 +239,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:t>Porcentagem</a:t>
+                  <a:t>Valores (%)</a:t>
                 </a:r>
               </a:p>
             </rich>

</xml_diff>